<commit_message>
Write up of results
</commit_message>
<xml_diff>
--- a/DataAnalysis.xlsx
+++ b/DataAnalysis.xlsx
@@ -9993,7 +9993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1011"/>
   <sheetViews>
-    <sheetView topLeftCell="I99" workbookViewId="0">
+    <sheetView topLeftCell="L131" workbookViewId="0">
       <selection activeCell="AD136" sqref="AD136"/>
     </sheetView>
   </sheetViews>
@@ -10019,7 +10019,7 @@
         <v>-9.9293753157590064E-2</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:U2" si="0">(B3+B104+B205+B306+B407+B508+B609+B710+B811+B912)/10</f>
+        <f t="shared" ref="L2:T2" si="0">(B3+B104+B205+B306+B407+B508+B609+B710+B811+B912)/10</f>
         <v>41.166666666666629</v>
       </c>
       <c r="M2">
@@ -10091,7 +10091,7 @@
         <v>-0.1107773592800028</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:U18" si="1">(B4+B105+B206+B307+B408+B509+B610+B711+B812+B913)/10</f>
+        <f t="shared" ref="L3:T18" si="1">(B4+B105+B206+B307+B408+B509+B610+B711+B812+B913)/10</f>
         <v>39.9</v>
       </c>
       <c r="M3">
@@ -14767,7 +14767,7 @@
         <v>2.5</v>
       </c>
       <c r="K68">
-        <f t="shared" ref="K68:K131" si="12">(A69+A170+A271+A372+A473+A574+A675+A776+A877+A978)/10</f>
+        <f t="shared" ref="K68:K101" si="12">(A69+A170+A271+A372+A473+A574+A675+A776+A877+A978)/10</f>
         <v>4.4863515116098325E-2</v>
       </c>
       <c r="L68">
@@ -46098,7 +46098,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>